<commit_message>
Fixed column name typos
</commit_message>
<xml_diff>
--- a/Statistical test and regression summaries/stat tests summary.xlsx
+++ b/Statistical test and regression summaries/stat tests summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\egyetem\hsdslab\twitter scraping\CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7487F5C4-68A6-4B49-9390-3B8531A37669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED04CC4D-B035-4AE9-BE1B-5E5B448601CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,9 +426,6 @@
     <t>is the mean greater in the category? / is the correlation positive?</t>
   </si>
   <si>
-    <t>top4 the mean greater in the category?  / is the correlation positive?</t>
-  </si>
-  <si>
     <t>Fisher exact tests for the odds ratio of a tweet becoming popular depending on the presence of a given category (one-vs-rest for higher cardinality). H0: the odds ratio is 1.</t>
   </si>
   <si>
@@ -463,6 +460,9 @@
   </si>
   <si>
     <t>(top4) probability of popular tweets in the rest</t>
+  </si>
+  <si>
+    <t>top4 is the mean greater in the category?  / is the correlation positive?</t>
   </si>
 </sst>
 </file>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F87" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
-      <selection activeCell="K118" sqref="K118"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -982,7 +982,7 @@
         <v>132</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>11</v>
@@ -5396,7 +5396,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B91" s="10"/>
       <c r="C91" s="10"/>
@@ -5434,7 +5434,7 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B93" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>2</v>
@@ -5446,37 +5446,37 @@
         <v>5</v>
       </c>
       <c r="F93" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="K93" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G93" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K93" s="1" t="s">
+      <c r="L93" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="L93" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="M93" s="1" t="s">
         <v>93</v>
       </c>
       <c r="N93" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O93" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="O93" s="1" t="s">
+      <c r="P93" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="P93" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.35">

</xml_diff>